<commit_message>
Edit name file, TC_ID, and Sheet name SCD0001 - SCD0009 && Fixing SCD0338-001
</commit_message>
<xml_diff>
--- a/Lib_Repo_Excel/FileExcel_Digisales/SCD0338-001 - View agenda pada Mobile.xlsx
+++ b/Lib_Repo_Excel/FileExcel_Digisales/SCD0338-001 - View agenda pada Mobile.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\1427\Documents\BNI\DigiSales\Lib_Repo_Excel\FileExcel_Digisales\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52FFA0A8-52BE-498D-BF26-887D904E3869}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{018835A7-5308-4D1B-BAE5-144AF97EF4F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="34">
   <si>
     <t>RUN</t>
   </si>
@@ -126,13 +126,19 @@
     <t>Follow Up</t>
   </si>
   <si>
-    <t>Test Daily Activity 2</t>
-  </si>
-  <si>
-    <t>03:50 PM</t>
-  </si>
-  <si>
-    <t>04:30 PM</t>
+    <t>08:50 PM</t>
+  </si>
+  <si>
+    <t>08:30 PM</t>
+  </si>
+  <si>
+    <t>10:00 PM</t>
+  </si>
+  <si>
+    <t>07:05 PM</t>
+  </si>
+  <si>
+    <t>Test Daily Activity 3</t>
   </si>
 </sst>
 </file>
@@ -540,8 +546,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0EAF5E5-8229-45B3-AC11-8AED029F52F4}">
   <dimension ref="A1:S7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F2" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="Q3" sqref="Q3"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="P3" sqref="P3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -654,20 +660,20 @@
         <v>24</v>
       </c>
       <c r="L2" s="13" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="M2" s="8" t="s">
         <v>25</v>
       </c>
       <c r="N2" s="15" t="str">
         <f ca="1">TEXT(TODAY(),"dd-mmm-yyyy")</f>
-        <v>21-Oct-2022</v>
+        <v>02-Nov-2022</v>
       </c>
       <c r="O2" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="P2" s="16" t="s">
         <v>30</v>
-      </c>
-      <c r="P2" s="16" t="s">
-        <v>31</v>
       </c>
       <c r="Q2" s="8" t="s">
         <v>27</v>
@@ -710,17 +716,17 @@
         <v>24</v>
       </c>
       <c r="L3" s="13" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="M3" s="8" t="s">
         <v>25</v>
       </c>
       <c r="N3" s="15" t="str">
         <f ca="1">TEXT(TODAY(),"dd-mmm-yyyy")</f>
-        <v>21-Oct-2022</v>
+        <v>02-Nov-2022</v>
       </c>
       <c r="O3" s="16" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="P3" s="16" t="s">
         <v>31</v>

</xml_diff>

<commit_message>
Fixing and re-run SCD0338-001 - SCD0338-014
</commit_message>
<xml_diff>
--- a/Lib_Repo_Excel/FileExcel_Digisales/SCD0338-001 - View agenda pada Mobile.xlsx
+++ b/Lib_Repo_Excel/FileExcel_Digisales/SCD0338-001 - View agenda pada Mobile.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\1427\Documents\BNI\DigiSales\Lib_Repo_Excel\FileExcel_Digisales\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{018835A7-5308-4D1B-BAE5-144AF97EF4F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1BC43BF-5DAA-4FA0-B246-D95EE9B09BE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -132,13 +132,13 @@
     <t>08:30 PM</t>
   </si>
   <si>
-    <t>10:00 PM</t>
-  </si>
-  <si>
     <t>07:05 PM</t>
   </si>
   <si>
-    <t>Test Daily Activity 3</t>
+    <t>10:30 PM</t>
+  </si>
+  <si>
+    <t>Test Daily Activity 5</t>
   </si>
 </sst>
 </file>
@@ -546,8 +546,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0EAF5E5-8229-45B3-AC11-8AED029F52F4}">
   <dimension ref="A1:S7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="P3" sqref="P3"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="Q3" sqref="Q3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -667,10 +667,10 @@
       </c>
       <c r="N2" s="15" t="str">
         <f ca="1">TEXT(TODAY(),"dd-mmm-yyyy")</f>
-        <v>02-Nov-2022</v>
+        <v>03-Nov-2022</v>
       </c>
       <c r="O2" s="16" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="P2" s="16" t="s">
         <v>30</v>
@@ -723,13 +723,13 @@
       </c>
       <c r="N3" s="15" t="str">
         <f ca="1">TEXT(TODAY(),"dd-mmm-yyyy")</f>
-        <v>02-Nov-2022</v>
+        <v>03-Nov-2022</v>
       </c>
       <c r="O3" s="16" t="s">
         <v>29</v>
       </c>
       <c r="P3" s="16" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="Q3" s="8" t="s">
         <v>28</v>

</xml_diff>